<commit_message>
add other bert model
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software\python\workground\tweet_sentiment_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C0D3F1-35DB-4C2F-905D-E7BFA9FC93BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD096A8-5CE1-41CF-AF4C-E6780F069ECF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CFBD6B1C-90EE-407F-934E-9DA405374D61}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>bert_case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,7 +61,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>use sentiment word frequency + learing rate decay:</t>
+    <t>use sentiment word frequency + word counts:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>use sentiment word frequency + learning rate decay:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A312599-9CE1-4A90-98DB-8FC6E4291EC3}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -497,6 +501,9 @@
       <c r="C6">
         <v>0.62581571309360295</v>
       </c>
+      <c r="D6">
+        <v>0.70199999999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -516,7 +523,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -542,6 +549,48 @@
       </c>
       <c r="C12">
         <v>0.62536166837874496</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0.61737329228550897</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>0.62109860854033605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>0.62598893967624802</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>0.60709525571029099</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>0.627169190381766</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>0.61413615973564695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tweet_roberta.ipynb in thinking folder
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software\python\workground\tweet_sentiment_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C847D8EB-71C3-484F-B90D-6E181E6C1612}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA717522-AE6A-4FD0-8E23-677E611406A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CFBD6B1C-90EE-407F-934E-9DA405374D61}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>bert_case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -138,6 +138,30 @@
   </si>
   <si>
     <t>roberta + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roberta-large + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. roberta + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer） 2.使用learing schedule 3.分开neutral、postive + negative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. roberta + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer） 2.使用learing schedule 3.focal loss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. roberta + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer） 2.使用learing schedule 3.focal loss 4.使用logit比较</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -145,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,13 +194,27 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,7 +231,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -201,6 +239,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -517,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A312599-9CE1-4A90-98DB-8FC6E4291EC3}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1053,6 +1112,208 @@
         <v>0.69485699999999995</v>
       </c>
     </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C49">
+        <v>32</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>0.67965100000000001</v>
+      </c>
+      <c r="F49">
+        <v>0.69377299999999997</v>
+      </c>
+      <c r="G49">
+        <v>0.68747199999999997</v>
+      </c>
+      <c r="H49">
+        <v>0.68759999999999999</v>
+      </c>
+      <c r="I49">
+        <v>0.68715400000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="7" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="6">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C51" s="7">
+        <v>64</v>
+      </c>
+      <c r="D51" s="7">
+        <v>5</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0.67642800000000003</v>
+      </c>
+      <c r="F51" s="7">
+        <v>0.69160100000000002</v>
+      </c>
+      <c r="G51" s="7">
+        <v>0.70302200000000004</v>
+      </c>
+      <c r="H51" s="7">
+        <v>0.70055800000000001</v>
+      </c>
+      <c r="I51" s="7">
+        <v>0.70146799999999998</v>
+      </c>
+      <c r="J51" s="7">
+        <f>AVERAGE(E51:I51)</f>
+        <v>0.69461539999999999</v>
+      </c>
+      <c r="K51" s="9">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="42" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C54">
+        <v>64</v>
+      </c>
+      <c r="D54">
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <v>0.68259400000000003</v>
+      </c>
+      <c r="F54">
+        <v>0.69777100000000003</v>
+      </c>
+      <c r="G54">
+        <v>0.69530400000000003</v>
+      </c>
+      <c r="H54">
+        <v>0.69847700000000001</v>
+      </c>
+      <c r="I54">
+        <v>0.69914699999999996</v>
+      </c>
+      <c r="J54" s="4">
+        <f>AVERAGE(E54:I54)</f>
+        <v>0.69465860000000001</v>
+      </c>
+      <c r="K54" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="7" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="6">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C55" s="7">
+        <v>64</v>
+      </c>
+      <c r="D55" s="7">
+        <v>5</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0.68771899999999997</v>
+      </c>
+      <c r="F55" s="7">
+        <v>0.69833299999999998</v>
+      </c>
+      <c r="G55" s="7">
+        <v>0.70306299999999999</v>
+      </c>
+      <c r="H55" s="7">
+        <v>0.70338900000000004</v>
+      </c>
+      <c r="I55" s="7">
+        <v>0.69980299999999995</v>
+      </c>
+      <c r="J55" s="7">
+        <f>AVERAGE(E55:I55)</f>
+        <v>0.6984613999999999</v>
+      </c>
+      <c r="K55" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="42" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C56">
+        <v>64</v>
+      </c>
+      <c r="D56">
+        <v>5</v>
+      </c>
+      <c r="E56">
+        <v>0.69647199999999998</v>
+      </c>
+      <c r="F56">
+        <v>0.69698499999999997</v>
+      </c>
+      <c r="G56">
+        <v>0.69439399999999996</v>
+      </c>
+      <c r="H56">
+        <v>0.693102</v>
+      </c>
+      <c r="I56">
+        <v>0.69685900000000001</v>
+      </c>
+      <c r="J56">
+        <f>AVERAGE(E56:I56)</f>
+        <v>0.69556239999999991</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add tpu py_file and data argumentation
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software\python\workground\tweet_sentiment_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201D7A24-A71F-4A97-9266-31A68ACB797C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F660D6-A95E-4790-939E-D5A14120852B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CFBD6B1C-90EE-407F-934E-9DA405374D61}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="47">
   <si>
     <t>bert_case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -198,6 +198,26 @@
   </si>
   <si>
     <t>power_iterations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. roberta + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer） 2.使用learing schedule 3.focal loss 4.使用logit比较 5.去除标点符号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. roberta + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer） 2.使用learing schedule 3.focal loss 4.使用logit比较 5.去除空格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. roberta + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer） 2.使用learing schedule 3.focal loss 4.使用logit比较 5.data argumentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. roberta + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer） 2.使用learing schedule 3.focal loss 4.使用logit比较 5.data argumentation(使用了数据预处理)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. roberta + 5-fold（使用别人的分词工具）+ conv1d（使用最后两层layer） 2.使用learing schedule 3.focal loss 4.使用logit比较 5.data argumentation(仅仅补充头部和尾部信息)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -615,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A312599-9CE1-4A90-98DB-8FC6E4291EC3}">
-  <dimension ref="A1:O86"/>
+  <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="J93" sqref="J93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2201,7 +2221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B81" s="2">
         <v>4.0000000000000003E-5</v>
       </c>
@@ -2240,7 +2260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B82" s="2">
         <v>4.0000000000000003E-5</v>
       </c>
@@ -2279,7 +2299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E83">
         <v>0.68908499999999995</v>
       </c>
@@ -2309,7 +2329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E84">
         <v>0.68845699999999999</v>
       </c>
@@ -2320,21 +2340,273 @@
         <v>0.69242499999999996</v>
       </c>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="42" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C86">
+        <v>64</v>
+      </c>
+      <c r="D86">
+        <v>5</v>
+      </c>
       <c r="E86">
-        <v>0.71082800000000002</v>
+        <v>0.64483199999999996</v>
       </c>
       <c r="F86">
-        <v>0.720441</v>
+        <v>0.65651300000000001</v>
       </c>
       <c r="G86">
-        <v>0.71965900000000005</v>
-      </c>
-      <c r="H86">
-        <v>0.72213099999999997</v>
-      </c>
-      <c r="I86">
-        <v>0.72244399999999998</v>
+        <v>0.65056899999999995</v>
+      </c>
+      <c r="J86">
+        <f t="shared" ref="J86:J91" si="2">AVERAGE(E86:I86)</f>
+        <v>0.65063799999999994</v>
+      </c>
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="L86" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M86">
+        <v>0.66300000000000003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="42" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B87" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C87">
+        <v>64</v>
+      </c>
+      <c r="D87">
+        <v>5</v>
+      </c>
+      <c r="E87">
+        <v>0.68095899999999998</v>
+      </c>
+      <c r="F87">
+        <v>0.69272599999999995</v>
+      </c>
+      <c r="G87">
+        <v>0.69733100000000003</v>
+      </c>
+      <c r="H87">
+        <v>0.69836799999999999</v>
+      </c>
+      <c r="I87">
+        <v>0.69530700000000001</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="2"/>
+        <v>0.69293820000000006</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="42" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B88" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C88">
+        <v>64</v>
+      </c>
+      <c r="D88">
+        <v>5</v>
+      </c>
+      <c r="E88">
+        <v>0.697824</v>
+      </c>
+      <c r="F88">
+        <v>0.71689599999999998</v>
+      </c>
+      <c r="G88">
+        <v>0.72333800000000004</v>
+      </c>
+      <c r="H88">
+        <v>0.72910399999999997</v>
+      </c>
+      <c r="I88">
+        <v>0.72910399999999997</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="2"/>
+        <v>0.71925320000000004</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="56" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89" s="2">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="C89">
+        <v>86</v>
+      </c>
+      <c r="D89">
+        <v>5</v>
+      </c>
+      <c r="E89">
+        <v>0.70022700000000004</v>
+      </c>
+      <c r="F89">
+        <v>0.72020099999999998</v>
+      </c>
+      <c r="G89">
+        <v>0.71912200000000004</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="2"/>
+        <v>0.71318333333333328</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M89">
+        <v>0.71199999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="56" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B90" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C90">
+        <v>96</v>
+      </c>
+      <c r="D90">
+        <v>5</v>
+      </c>
+      <c r="E90">
+        <v>0.69025599999999998</v>
+      </c>
+      <c r="F90">
+        <v>0.70514100000000002</v>
+      </c>
+      <c r="G90">
+        <v>0.71001999999999998</v>
+      </c>
+      <c r="H90">
+        <v>0.71414599999999995</v>
+      </c>
+      <c r="I90">
+        <v>0.71295600000000003</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="2"/>
+        <v>0.70650380000000002</v>
+      </c>
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="L90" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M90">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="42" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B91" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="C91">
+        <v>96</v>
+      </c>
+      <c r="D91">
+        <v>5</v>
+      </c>
+      <c r="E91">
+        <v>0.68267100000000003</v>
+      </c>
+      <c r="F91">
+        <v>0.69822499999999998</v>
+      </c>
+      <c r="G91">
+        <v>0.69930700000000001</v>
+      </c>
+      <c r="H91">
+        <v>0.70250299999999999</v>
+      </c>
+      <c r="I91">
+        <v>0.70250299999999999</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="2"/>
+        <v>0.69704180000000004</v>
+      </c>
+      <c r="K91">
+        <v>1</v>
+      </c>
+      <c r="L91" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>